<commit_message>
Included testng execution .xml files
</commit_message>
<xml_diff>
--- a/src/test/resources/dataRepo/InputDataNew.xlsx
+++ b/src/test/resources/dataRepo/InputDataNew.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARUN\VtigerCRM\SDET37\src\test\resources\dataRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24184F3-EFD7-4792-AD08-F6586484A4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0F3BA2-EE1C-4C80-BC12-5F863FF63518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="9" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3384" yWindow="3360" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateProject" sheetId="1" r:id="rId1"/>
@@ -1782,7 +1782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B3515E8-37C2-4296-A442-F80CCC74F8D5}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1889,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C86E1374-09C6-41EE-923D-F04164B8E5DD}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>